<commit_message>
feat: adicionando planilha unificada
</commit_message>
<xml_diff>
--- a/2.3A - 4 - ver2.xlsx
+++ b/2.3A - 4 - ver2.xlsx
@@ -5,33 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsm44\Desktop\trabalhoPO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\trabalhoPO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE431D8E-1789-4151-BF7D-CEF99C052E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4622489-2B64-4BB9-99C2-B86524266534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EXERCICIO4 - 2.3A" sheetId="3" r:id="rId1"/>
+    <sheet name="2.3A" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$B$19:$H$19</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'2.3A'!$B$19:$H$19</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$B$19:$E$19</definedName>
-    <definedName name="solver_lhs10" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$18</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$B$19:$E$19</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$B$19:$H$19</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$F$19</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$G$19</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$G$19</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$G$19</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$H$19</definedName>
-    <definedName name="solver_lhs9" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$I$16</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'2.3A'!$B$19:$E$19</definedName>
+    <definedName name="solver_lhs10" localSheetId="0" hidden="1">'2.3A'!$K$18</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'2.3A'!$B$19:$E$19</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'2.3A'!$B$19:$H$19</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'2.3A'!$F$19</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'2.3A'!$G$19</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'2.3A'!$G$19</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">'2.3A'!$G$19</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">'2.3A'!$H$19</definedName>
+    <definedName name="solver_lhs9" localSheetId="0" hidden="1">'2.3A'!$I$16</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -41,7 +41,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">10</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$I$2</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'2.3A'!$I$2</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
@@ -54,16 +54,16 @@
     <definedName name="solver_rel7" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$3:$K$6</definedName>
-    <definedName name="solver_rhs10" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$17</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$11:$K$14</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'2.3A'!$K$3:$K$6</definedName>
+    <definedName name="solver_rhs10" localSheetId="0" hidden="1">'2.3A'!$K$17</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'2.3A'!$K$11:$K$14</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">"número inteiro"</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$8</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$15</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$9</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$7</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$10</definedName>
-    <definedName name="solver_rhs9" localSheetId="0" hidden="1">'EXERCICIO4 - 2.3A'!$K$16</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'2.3A'!$K$8</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">'2.3A'!$K$15</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">'2.3A'!$K$9</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">'2.3A'!$K$7</definedName>
+    <definedName name="solver_rhs8" localSheetId="0" hidden="1">'2.3A'!$K$10</definedName>
+    <definedName name="solver_rhs9" localSheetId="0" hidden="1">'2.3A'!$K$16</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -80,30 +80,19 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -353,12 +342,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color theme="2" tint="-0.24994659260841701"/>
@@ -642,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A36C73D-5DDD-4F70-818B-6E24CF2FC329}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,11 +1471,6 @@
     <mergeCell ref="P9:Q9"/>
     <mergeCell ref="P7:Q7"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:H15">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B2:H16">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>

</xml_diff>